<commit_message>
Rubriken überarbeitet, u. a. Rubrik "Handy" aufgenommen
</commit_message>
<xml_diff>
--- a/Jenzen/rubriken.xlsx
+++ b/Jenzen/rubriken.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
   <si>
     <t>Rubriken</t>
   </si>
@@ -121,16 +121,59 @@
   </si>
   <si>
     <t>pc</t>
+  </si>
+  <si>
+    <t>PC Server</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>Arbeit</t>
+  </si>
+  <si>
+    <t>Haus</t>
+  </si>
+  <si>
+    <t>KFZ</t>
+  </si>
+  <si>
+    <t>Kinder</t>
+  </si>
+  <si>
+    <t>Korr. Faktor</t>
+  </si>
+  <si>
+    <t>Kleidung</t>
+  </si>
+  <si>
+    <t>Hauskosten variabel (Baumarkt, IKEA)</t>
+  </si>
+  <si>
+    <t>KFZ Kosten variabel, ohne Versicherung + Tanken</t>
+  </si>
+  <si>
+    <t>Leben täglicher Bedarf (Einkauf, Körperpflege, etc)</t>
+  </si>
+  <si>
+    <t>handy</t>
+  </si>
+  <si>
+    <t>Handy Susi, Matz, Marlena, Finn</t>
+  </si>
+  <si>
+    <t>Korrektur Betrag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,8 +513,44 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCDCD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0EBB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE697"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE79B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -586,8 +665,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -631,8 +719,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,9 +732,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -653,26 +739,107 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+  <cellStyles count="44">
+    <cellStyle name="20% - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -681,6 +848,7 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Dezimal" xfId="43" builtinId="3"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -699,8 +867,181 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD0EBB3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD0EBB3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD0EBB3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD0EBB3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE79B"/>
+      <color rgb="FFFFFFC1"/>
+      <color rgb="FFFFE697"/>
+      <color rgb="FFFFCDCD"/>
+      <color rgb="FFD0EBB3"/>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -710,7 +1051,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -784,7 +1125,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -819,7 +1159,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -995,27 +1334,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="43.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1029,7 +1368,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1396,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" s="3" customFormat="1">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1071,7 +1410,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1085,7 +1424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" s="3" customFormat="1">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1433,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1453,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1122,7 +1461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1130,7 +1469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1138,7 +1477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
@@ -1153,275 +1492,572 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="5"/>
-    <col min="2" max="2" width="11.42578125" style="7"/>
-    <col min="3" max="3" width="11.42578125" style="4"/>
-    <col min="7" max="7" width="11.42578125" style="8"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="6"/>
+    <col min="4" max="4" width="48" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="7"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="F1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="22">
         <v>2014</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4">
         <v>-154.30000000000001</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="16">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <f>E2*F2</f>
+        <v>-154.30000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-808.33330000000001</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ref="G3:G6" si="0">E3*F3</f>
+        <v>-727.49997000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4">
+        <f>-988.9808-E10</f>
+        <v>-912.98080000000004</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="0"/>
+        <v>-821.68272000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-29.166599999999999</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-39.99</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="37">
+        <v>2014</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-333.92160000000001</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="13">
+        <f>E7*F7</f>
+        <v>-100.17648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="37">
+        <v>2014</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-974.38660000000004</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="13">
+        <f>E8*F8</f>
+        <v>-779.5092800000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="40">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="43">
+        <v>-263.45659999999998</v>
+      </c>
+      <c r="F9" s="44">
+        <v>1</v>
+      </c>
+      <c r="G9" s="45">
+        <f>E9*F9</f>
+        <v>-263.45659999999998</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1">
+      <c r="A10" s="40">
+        <v>2014</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="4">
+        <v>-76</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="13">
+        <f>E10*F10</f>
+        <v>-38</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="31">
+        <v>2014</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-604.70579999999995</v>
+      </c>
+      <c r="F11" s="16">
+        <v>2</v>
+      </c>
+      <c r="G11" s="13">
+        <f>E11*F11</f>
+        <v>-1209.4115999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="28">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-524.85249999999996</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" ref="G12" si="1">E12*F12</f>
+        <v>-524.85249999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="28">
+        <v>2014</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-203.47579999999999</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
+        <f>E13*F13</f>
+        <v>-203.47579999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="19">
+        <v>2014</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-123.0116</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="G14" s="13">
+        <f>E14*F14</f>
+        <v>-153.7645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="19">
+        <v>2014</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-79.287499999999994</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13">
+        <f>E15*F15</f>
+        <v>-79.287499999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="34">
+        <v>2014</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="12">
+        <v>-155.19829999999999</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <f>E16*F16</f>
+        <v>-155.19829999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11">
+      <c r="E17" s="9">
+        <f>SUM(E2:E16)</f>
+        <v>-5283.0670000000009</v>
+      </c>
+      <c r="G17" s="9">
+        <f>SUM(G2:G16)</f>
+        <v>-5210.6152500000007</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="5:11">
+      <c r="I18" s="8"/>
+    </row>
+    <row r="20" spans="5:11">
+      <c r="I20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="5:11">
+      <c r="I21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4">
-        <v>-808.33330000000001</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="5:11">
+      <c r="I22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4">
-        <v>-988.98080000000004</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="5:11">
+      <c r="I23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4">
-        <v>-29.166599999999999</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="5:11">
+      <c r="I24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4">
-        <v>-524.85249999999996</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-203.47579999999999</v>
-      </c>
-      <c r="G7" s="9" t="s">
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="5:11">
+      <c r="I25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>-123.0116</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="5:11">
+      <c r="I26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4">
-        <v>-604.70579999999995</v>
-      </c>
-      <c r="G9" s="9" t="s">
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="5:11">
+      <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4">
-        <v>-333.92160000000001</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="5:11">
+      <c r="I28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4">
-        <v>-79.287499999999994</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="5:11">
+      <c r="I29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4">
-        <v>-974.38660000000004</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="5:11">
+      <c r="I30" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="5:11">
+      <c r="I31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="5:11">
+      <c r="I32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="4">
-        <v>-39.99</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
-        <v>-155.19829999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>2014</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>-263.45659999999998</v>
-      </c>
+      <c r="J32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="G2:H13">
-    <sortCondition ref="G2"/>
+  <sortState ref="A2:F16">
+    <sortCondition ref="B2:B16"/>
   </sortState>
+  <conditionalFormatting sqref="F2:F16">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>$E2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="greaterThan">
+      <formula>$E2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>